<commit_message>
Update in bench mark and optimization
</commit_message>
<xml_diff>
--- a/Source/Example Measurements/Image rendering/Image_Transfer_BenchMark.xlsx
+++ b/Source/Example Measurements/Image rendering/Image_Transfer_BenchMark.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Image Transfer to IS" sheetId="1" r:id="rId1"/>
+    <sheet name="Image Streaming" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="27">
   <si>
     <t>S.NO</t>
   </si>
@@ -72,6 +73,36 @@
   </si>
   <si>
     <t>Image 2D pixel array to 1D array</t>
+  </si>
+  <si>
+    <t>Json string</t>
+  </si>
+  <si>
+    <t>CSV string</t>
+  </si>
+  <si>
+    <t>1D array</t>
+  </si>
+  <si>
+    <t>Compressed string to byte array</t>
+  </si>
+  <si>
+    <t>7.4 ms</t>
+  </si>
+  <si>
+    <t>1280x720</t>
+  </si>
+  <si>
+    <t>U32 1D array</t>
+  </si>
+  <si>
+    <t>14 ms</t>
+  </si>
+  <si>
+    <t>1 sec</t>
+  </si>
+  <si>
+    <t>Time Taken for sending each frame of image</t>
   </si>
 </sst>
 </file>
@@ -193,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -232,6 +263,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -264,6 +298,40 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Time to transfer the Image data to UI (s)</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Json string approach</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -295,9 +363,48 @@
       </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
+      <c:bar3DChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
@@ -306,14 +413,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Image Transfer to IS'!$C$6:$D$6</c:f>
+              <c:f>'Image Transfer to IS'!$E$13</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>329.15 KB</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1920x1080</c:v>
+                  <c:v>Time to taken to transfer the Image data to UI (s)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -326,9 +430,79 @@
               <a:noFill/>
             </a:ln>
             <a:effectLst/>
+            <a:sp3d/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-4.1666666666666755E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-DCD9-4FE4-9D4B-A7B506C901A8}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.7777777777777779E-3"/>
+                  <c:y val="-3.2407407407407489E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-DCD9-4FE4-9D4B-A7B506C901A8}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.777777777777676E-3"/>
+                  <c:y val="-3.2407407407407406E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-DCD9-4FE4-9D4B-A7B506C901A8}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -358,7 +532,6 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -387,252 +560,48 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Image Transfer to IS'!$D$14:$D$16</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1920x1080</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6000x4000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7360x4912</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Image Transfer to IS'!$E$6:$G$6</c:f>
+              <c:f>'Image Transfer to IS'!$E$14:$E$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1.4641999999999999</c:v>
+                  <c:v>0.69374999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0548999999999999</c:v>
+                  <c:v>7.6021000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0965500000000001</c:v>
+                  <c:v>16.98415</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F621-48D3-A4E7-932522AFB3C2}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Image Transfer to IS'!$C$7:$D$7</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>11.3 MB</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6000x4000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>'Image Transfer to IS'!$E$7:$G$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>15.453099999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>16.15775</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>17.804650000000002</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-F621-48D3-A4E7-932522AFB3C2}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Image Transfer to IS'!$C$8:$D$8</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>43.8 MB</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7360x4912</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>'Image Transfer to IS'!$E$8:$G$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>28.259149999999998</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>24.398499999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>26.2974</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-F621-48D3-A4E7-932522AFB3C2}"/>
+              <c16:uniqueId val="{00000000-DCD9-4FE4-9D4B-A7B506C901A8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
@@ -640,138 +609,19 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="383127016"/>
-        <c:axId val="383128656"/>
-      </c:barChart>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="504014120"/>
+        <c:axId val="497640728"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
       <c:catAx>
-        <c:axId val="383127016"/>
+        <c:axId val="504014120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="383128656"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="383128656"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Time (s)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -803,7 +653,67 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="383127016"/>
+        <c:crossAx val="497640728"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="497640728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="20"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="504014120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -815,8 +725,102 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Time to transfer the Image data to UI (s)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>CSV string approach</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -831,7 +835,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -846,7 +850,836 @@
           <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
-    </c:legend>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.5462668816039986E-17"/>
+                  <c:y val="-9.2592592592592587E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-A5D0-42AF-A3EA-3C073DCA9F7A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="5.5555555555555558E-3"/>
+                  <c:y val="-0.25"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-A5D0-42AF-A3EA-3C073DCA9F7A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.0185067526415994E-16"/>
+                  <c:y val="-0.33796296296296302"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-A5D0-42AF-A3EA-3C073DCA9F7A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Image Transfer to IS'!$D$17:$D$19</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1920x1080</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6000x4000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7360x4912</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Image Transfer to IS'!$E$17:$E$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.0548999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.15775</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.398499999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A5D0-42AF-A3EA-3C073DCA9F7A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="501050384"/>
+        <c:axId val="501050712"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="501050384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="501050712"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="501050712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="501050384"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Time to transfer the Image data to UI (s)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>1D array approach</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.5555555555555558E-3"/>
+                  <c:y val="-7.407407407407407E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-29D5-45EA-9619-51D071076853}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.3333333333333332E-3"/>
+                  <c:y val="-8.7962962962962965E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-29D5-45EA-9619-51D071076853}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.3333333333333332E-3"/>
+                  <c:y val="-9.2592592592592671E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-29D5-45EA-9619-51D071076853}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Image Transfer to IS'!$D$20:$D$22</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1920x1080</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6000x4000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7360x4912</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Image Transfer to IS'!$E$20:$E$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.1978</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.98170000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5390000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-29D5-45EA-9619-51D071076853}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="456747368"/>
+        <c:axId val="456748024"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="456747368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="456748024"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="456748024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="20"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="456747368"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -924,8 +1757,88 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -948,17 +1861,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
@@ -1129,22 +2031,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -1249,8 +2152,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1382,19 +2285,1008 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1431,20 +3323,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>4762</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1443037</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="6" name="Chart 5"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1454,6 +3346,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1471612</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1262062</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1300162</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>109537</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1725,10 +3677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I13"/>
+  <dimension ref="B2:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2029,16 +3981,199 @@
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E13" s="2"/>
+    <row r="13" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="5">
+        <f>(0.6355+0.752)/2</f>
+        <v>0.69374999999999998</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="7">
+        <f>(7.3949+7.8093)/2</f>
+        <v>7.6021000000000001</v>
+      </c>
+      <c r="F15" s="12"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D16" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="9">
+        <f>(20.5885+13.3798)/2</f>
+        <v>16.98415</v>
+      </c>
+      <c r="F16" s="13"/>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="5">
+        <f>(1.0358+1.074)/2</f>
+        <v>1.0548999999999999</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D18" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="7">
+        <f>(17.2829+15.0326)/2</f>
+        <v>16.15775</v>
+      </c>
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D19" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="9">
+        <f>(26.4147+22.3823)/2</f>
+        <v>24.398499999999999</v>
+      </c>
+      <c r="F19" s="13"/>
+    </row>
+    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="5">
+        <f>(0.2024+0.1932)/2</f>
+        <v>0.1978</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D21" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="7">
+        <f>(0.9908+0.9726)/2</f>
+        <v>0.98170000000000002</v>
+      </c>
+      <c r="F21" s="14"/>
+    </row>
+    <row r="22" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D22" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="9">
+        <f>(1.5498+1.5282)/2</f>
+        <v>1.5390000000000001</v>
+      </c>
+      <c r="F22" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
+    <mergeCell ref="F20:F22"/>
     <mergeCell ref="I3:I5"/>
     <mergeCell ref="I6:I8"/>
     <mergeCell ref="I9:I11"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="F17:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="26" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="16">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="16">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="16">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Document update and clean up
</commit_message>
<xml_diff>
--- a/Source/Example Measurements/Image rendering/Image_Transfer_BenchMark.xlsx
+++ b/Source/Example Measurements/Image rendering/Image_Transfer_BenchMark.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="32">
   <si>
     <t>S.NO</t>
   </si>
@@ -96,13 +96,28 @@
     <t>U32 1D array</t>
   </si>
   <si>
-    <t>14 ms</t>
+    <t>10 ms</t>
   </si>
   <si>
-    <t>1 sec</t>
+    <t>Comment</t>
   </si>
   <si>
-    <t>Time Taken for sending each frame of image</t>
+    <t>30 fps</t>
+  </si>
+  <si>
+    <t>15 ms</t>
+  </si>
+  <si>
+    <t>Average Time Taken for sending each frame of image</t>
+  </si>
+  <si>
+    <t>75ms</t>
+  </si>
+  <si>
+    <t>30 ms</t>
+  </si>
+  <si>
+    <t>1.3 s</t>
   </si>
 </sst>
 </file>
@@ -224,7 +239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -248,13 +263,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -263,8 +275,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -541,7 +559,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1019,7 +1036,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1496,7 +1512,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3679,8 +3694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3746,7 +3761,7 @@
         <f>SUM(E3:G3)</f>
         <v>2.3969500000000004</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="12" t="s">
         <v>14</v>
       </c>
     </row>
@@ -3776,7 +3791,7 @@
         <f>SUM(E4:G4)</f>
         <v>99.48214999999999</v>
       </c>
-      <c r="I4" s="12"/>
+      <c r="I4" s="15"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="8">
@@ -3804,7 +3819,7 @@
         <f>SUM(E5:G5)</f>
         <v>106.089</v>
       </c>
-      <c r="I5" s="13"/>
+      <c r="I5" s="16"/>
     </row>
     <row r="6" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
@@ -3832,7 +3847,7 @@
         <f t="shared" ref="H6:H11" si="0">SUM(E6:G6)</f>
         <v>3.61565</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="12" t="s">
         <v>13</v>
       </c>
     </row>
@@ -3862,7 +3877,7 @@
         <f t="shared" si="0"/>
         <v>49.415500000000002</v>
       </c>
-      <c r="I7" s="12"/>
+      <c r="I7" s="15"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="8">
@@ -3890,7 +3905,7 @@
         <f t="shared" si="0"/>
         <v>78.95505</v>
       </c>
-      <c r="I8" s="13"/>
+      <c r="I8" s="16"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
@@ -3918,7 +3933,7 @@
         <f t="shared" si="0"/>
         <v>1.4319</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="I9" s="12" t="s">
         <v>16</v>
       </c>
     </row>
@@ -3948,7 +3963,7 @@
         <f>SUM(E10:G10)</f>
         <v>21.130800000000001</v>
       </c>
-      <c r="I10" s="14"/>
+      <c r="I10" s="13"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="8">
@@ -3976,7 +3991,7 @@
         <f t="shared" si="0"/>
         <v>34.38805</v>
       </c>
-      <c r="I11" s="15"/>
+      <c r="I11" s="14"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E12" s="2"/>
@@ -4000,7 +4015,7 @@
         <f>(0.6355+0.752)/2</f>
         <v>0.69374999999999998</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F14" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -4012,7 +4027,7 @@
         <f>(7.3949+7.8093)/2</f>
         <v>7.6021000000000001</v>
       </c>
-      <c r="F15" s="12"/>
+      <c r="F15" s="15"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D16" s="9" t="s">
@@ -4022,7 +4037,7 @@
         <f>(20.5885+13.3798)/2</f>
         <v>16.98415</v>
       </c>
-      <c r="F16" s="13"/>
+      <c r="F16" s="16"/>
     </row>
     <row r="17" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D17" s="5" t="s">
@@ -4032,7 +4047,7 @@
         <f>(1.0358+1.074)/2</f>
         <v>1.0548999999999999</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="12" t="s">
         <v>18</v>
       </c>
     </row>
@@ -4044,7 +4059,7 @@
         <f>(17.2829+15.0326)/2</f>
         <v>16.15775</v>
       </c>
-      <c r="F18" s="12"/>
+      <c r="F18" s="15"/>
     </row>
     <row r="19" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D19" s="9" t="s">
@@ -4054,7 +4069,7 @@
         <f>(26.4147+22.3823)/2</f>
         <v>24.398499999999999</v>
       </c>
-      <c r="F19" s="13"/>
+      <c r="F19" s="16"/>
     </row>
     <row r="20" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D20" s="5" t="s">
@@ -4064,7 +4079,7 @@
         <f>(0.2024+0.1932)/2</f>
         <v>0.1978</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F20" s="12" t="s">
         <v>19</v>
       </c>
     </row>
@@ -4076,7 +4091,7 @@
         <f>(0.9908+0.9726)/2</f>
         <v>0.98170000000000002</v>
       </c>
-      <c r="F21" s="14"/>
+      <c r="F21" s="13"/>
     </row>
     <row r="22" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D22" s="9" t="s">
@@ -4086,7 +4101,7 @@
         <f>(1.5498+1.5282)/2</f>
         <v>1.5390000000000001</v>
       </c>
-      <c r="F22" s="15"/>
+      <c r="F22" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -4104,10 +4119,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E5"/>
+  <dimension ref="B2:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4115,9 +4130,10 @@
     <col min="3" max="3" width="17.5703125" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
     <col min="5" max="5" width="30.7109375" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -4125,14 +4141,17 @@
         <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="16">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="11">
         <v>1</v>
       </c>
       <c r="C3" t="s">
@@ -4144,36 +4163,89 @@
       <c r="E3" t="s">
         <v>20</v>
       </c>
+      <c r="F3" s="17" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="16">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="11">
         <v>2</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
         <v>23</v>
       </c>
+      <c r="F4" s="17"/>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="16">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="11">
         <v>3</v>
       </c>
       <c r="C5" t="s">
         <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
         <v>17</v>
       </c>
+      <c r="F5" s="17"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="11">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="17"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="11">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="17"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="11">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="17"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F3:F8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update in bench mark value
</commit_message>
<xml_diff>
--- a/Source/Example Measurements/Image rendering/Image_Transfer_BenchMark.xlsx
+++ b/Source/Example Measurements/Image rendering/Image_Transfer_BenchMark.xlsx
@@ -87,16 +87,10 @@
     <t>Compressed string to byte array</t>
   </si>
   <si>
-    <t>7.4 ms</t>
-  </si>
-  <si>
     <t>1280x720</t>
   </si>
   <si>
     <t>U32 1D array</t>
-  </si>
-  <si>
-    <t>10 ms</t>
   </si>
   <si>
     <t>Comment</t>
@@ -105,19 +99,25 @@
     <t>30 fps</t>
   </si>
   <si>
-    <t>15 ms</t>
-  </si>
-  <si>
     <t>Average Time Taken for sending each frame of image</t>
   </si>
   <si>
-    <t>75ms</t>
+    <t>1.3 s</t>
   </si>
   <si>
-    <t>30 ms</t>
+    <t>74 ms</t>
   </si>
   <si>
-    <t>1.3 s</t>
+    <t>150 ms</t>
+  </si>
+  <si>
+    <t>750 ms</t>
+  </si>
+  <si>
+    <t>100 ms</t>
+  </si>
+  <si>
+    <t>300 ms</t>
   </si>
 </sst>
 </file>
@@ -4122,7 +4122,7 @@
   <dimension ref="B2:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4141,13 +4141,13 @@
         <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -4155,16 +4155,16 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
         <v>20</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
@@ -4172,13 +4172,13 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
         <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
       </c>
       <c r="F4" s="17"/>
     </row>
@@ -4187,7 +4187,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
         <v>29</v>
@@ -4205,7 +4205,7 @@
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E6" t="s">
         <v>20</v>
@@ -4220,10 +4220,10 @@
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7" s="17"/>
     </row>
@@ -4235,7 +4235,7 @@
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
         <v>17</v>

</xml_diff>